<commit_message>
Make phone list reading more robust; fix spreadsheet errors
</commit_message>
<xml_diff>
--- a/report/Debug/phone_list.xlsx
+++ b/report/Debug/phone_list.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="314">
   <si>
     <t>ASSISTANTS</t>
   </si>
@@ -946,6 +946,21 @@
   </si>
   <si>
     <t>TOUR_S</t>
+  </si>
+  <si>
+    <t>Phone number</t>
+  </si>
+  <si>
+    <t>Short name</t>
+  </si>
+  <si>
+    <t>Zone</t>
+  </si>
+  <si>
+    <t>Long name</t>
+  </si>
+  <si>
+    <t>English unit</t>
   </si>
 </sst>
 </file>
@@ -1753,1635 +1768,1654 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N101"/>
+  <dimension ref="A1:O102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="9.140625" style="1"/>
-    <col min="7" max="11" width="9.140625" style="1"/>
-    <col min="13" max="13" width="9.140625" style="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="4" width="31.85546875" style="1" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="1"/>
+    <col min="8" max="12" width="9.140625" style="1"/>
+    <col min="14" max="14" width="9.140625" style="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="G1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G2" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="1"/>
-      <c r="N1" s="1"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="M2" s="1"/>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G3" t="s">
         <v>87</v>
       </c>
-      <c r="L2" s="1"/>
-      <c r="N2" s="1"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="M3" s="1"/>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G4" t="s">
         <v>88</v>
       </c>
-      <c r="L3" s="1"/>
-      <c r="N3" s="1"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="M4" s="1"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G5" t="s">
         <v>89</v>
       </c>
-      <c r="L4" s="1"/>
-      <c r="N4" s="1"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="M5" s="1"/>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G6" t="s">
         <v>90</v>
       </c>
-      <c r="L5" s="1"/>
-      <c r="N5" s="1"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="M6" s="1"/>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G7" t="s">
         <v>91</v>
       </c>
-      <c r="L6" s="1"/>
-      <c r="N6" s="1"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="M7" s="1"/>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G8" t="s">
         <v>92</v>
       </c>
-      <c r="L7" s="1"/>
-      <c r="N7" s="1"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="M8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G9" t="s">
         <v>93</v>
       </c>
-      <c r="L8" s="1"/>
-      <c r="N8" s="1"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="M9" s="1"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G10" t="s">
         <v>94</v>
       </c>
-      <c r="L9" s="1"/>
-      <c r="N9" s="1"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="M10" s="1"/>
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G11" t="s">
         <v>95</v>
       </c>
-      <c r="L10" s="1"/>
-      <c r="N10" s="1"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="M11" s="1"/>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G12" t="s">
         <v>96</v>
       </c>
-      <c r="L11" s="1"/>
-      <c r="N11" s="1"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="M12" s="1"/>
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G13" t="s">
         <v>97</v>
       </c>
-      <c r="L12" s="1"/>
-      <c r="N12" s="1"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="M13" s="1"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G14" t="s">
         <v>98</v>
       </c>
-      <c r="L13" s="1"/>
-      <c r="N13" s="1"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="M14" s="1"/>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G15" t="s">
         <v>99</v>
       </c>
-      <c r="L14" s="1"/>
-      <c r="N14" s="1"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="M15" s="1"/>
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G16" t="s">
         <v>100</v>
       </c>
-      <c r="L15" s="1"/>
-      <c r="N15" s="1"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="M16" s="1"/>
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G17" t="s">
         <v>101</v>
       </c>
-      <c r="L16" s="1"/>
-      <c r="N16" s="1"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="M17" s="1"/>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G18" t="s">
         <v>102</v>
       </c>
-      <c r="L17" s="1"/>
-      <c r="N17" s="1"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="M18" s="1"/>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G19" t="s">
         <v>104</v>
       </c>
-      <c r="L18" s="1"/>
-      <c r="N18" s="1"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="M19" s="1"/>
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G20" t="s">
         <v>105</v>
       </c>
-      <c r="L19" s="1"/>
-      <c r="N19" s="1"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="M20" s="1"/>
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G21" t="s">
         <v>106</v>
       </c>
-      <c r="L20" s="1"/>
-      <c r="N20" s="1"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="M21" s="1"/>
+      <c r="O21" s="1"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G22" t="s">
         <v>107</v>
       </c>
-      <c r="L21" s="1"/>
-      <c r="N21" s="1"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="M22" s="1"/>
+      <c r="O22" s="1"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G23" t="s">
         <v>108</v>
       </c>
-      <c r="L22" s="1"/>
-      <c r="N22" s="1"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="M23" s="1"/>
+      <c r="O23" s="1"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G24" t="s">
         <v>109</v>
       </c>
-      <c r="L23" s="1"/>
-      <c r="N23" s="1"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="M24" s="1"/>
+      <c r="O24" s="1"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G25" t="s">
         <v>110</v>
       </c>
-      <c r="L24" s="1"/>
-      <c r="N24" s="1"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="M25" s="1"/>
+      <c r="O25" s="1"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G26" t="s">
         <v>111</v>
       </c>
-      <c r="L25" s="1"/>
-      <c r="N25" s="1"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="M26" s="1"/>
+      <c r="O26" s="1"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G27" t="s">
         <v>112</v>
       </c>
-      <c r="L26" s="1"/>
-      <c r="N26" s="1"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="M27" s="1"/>
+      <c r="O27" s="1"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G28" t="s">
         <v>113</v>
       </c>
-      <c r="L27" s="1"/>
-      <c r="N27" s="1"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="M28" s="1"/>
+      <c r="O28" s="1"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G29" t="s">
         <v>115</v>
       </c>
-      <c r="L28" s="1"/>
-      <c r="N28" s="1"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="M29" s="1"/>
+      <c r="O29" s="1"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G30" t="s">
         <v>116</v>
       </c>
-      <c r="L29" s="1"/>
-      <c r="N29" s="1"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="M30" s="1"/>
+      <c r="O30" s="1"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G31" t="s">
         <v>117</v>
       </c>
-      <c r="L30" s="1"/>
-      <c r="N30" s="1"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="M31" s="1"/>
+      <c r="O31" s="1"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G32" t="s">
         <v>118</v>
       </c>
-      <c r="L31" s="1"/>
-      <c r="N31" s="1"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="M32" s="1"/>
+      <c r="O32" s="1"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G33" t="s">
         <v>119</v>
       </c>
-      <c r="L32" s="1"/>
-      <c r="N32" s="1"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="M33" s="1"/>
+      <c r="O33" s="1"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G34" t="s">
         <v>120</v>
       </c>
-      <c r="L33" s="1"/>
-      <c r="N33" s="1"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="M34" s="1"/>
+      <c r="O34" s="1"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G35" t="s">
         <v>121</v>
       </c>
-      <c r="L34" s="1"/>
-      <c r="N34" s="1"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="M35" s="1"/>
+      <c r="O35" s="1"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G36" t="s">
         <v>123</v>
       </c>
-      <c r="L35" s="1"/>
-      <c r="N35" s="1"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="M36" s="1"/>
+      <c r="O36" s="1"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G37" t="s">
         <v>124</v>
       </c>
-      <c r="L36" s="1"/>
-      <c r="N36" s="1"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="M37" s="1"/>
+      <c r="O37" s="1"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G38" t="s">
         <v>125</v>
       </c>
-      <c r="L37" s="1"/>
-      <c r="N37" s="1"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="M38" s="1"/>
+      <c r="O38" s="1"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G39" t="s">
         <v>126</v>
       </c>
-      <c r="L38" s="1"/>
-      <c r="N38" s="1"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="M39" s="1"/>
+      <c r="O39" s="1"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G40" t="s">
         <v>127</v>
       </c>
-      <c r="L39" s="1"/>
-      <c r="N39" s="1"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="M40" s="1"/>
+      <c r="O40" s="1"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G41" t="s">
         <v>128</v>
       </c>
-      <c r="L40" s="1"/>
-      <c r="N40" s="1"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="M41" s="1"/>
+      <c r="O41" s="1"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G42" t="s">
         <v>129</v>
       </c>
-      <c r="L41" s="1"/>
-      <c r="N41" s="1"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="M42" s="1"/>
+      <c r="O42" s="1"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G43" t="s">
         <v>131</v>
       </c>
-      <c r="L42" s="1"/>
-      <c r="N42" s="1"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="M43" s="1"/>
+      <c r="O43" s="1"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G44" t="s">
         <v>132</v>
       </c>
-      <c r="L43" s="1"/>
-      <c r="N43" s="1"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="M44" s="1"/>
+      <c r="O44" s="1"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G45" t="s">
         <v>133</v>
       </c>
-      <c r="L44" s="1"/>
-      <c r="N44" s="1"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="M45" s="1"/>
+      <c r="O45" s="1"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F45" t="s">
+      <c r="G46" t="s">
         <v>134</v>
       </c>
-      <c r="L45" s="1"/>
-      <c r="N45" s="1"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="M46" s="1"/>
+      <c r="O46" s="1"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="F47" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G47" t="s">
         <v>135</v>
       </c>
-      <c r="L46" s="1"/>
-      <c r="N46" s="1"/>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="M47" s="1"/>
+      <c r="O47" s="1"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F47" t="s">
+      <c r="G48" t="s">
         <v>136</v>
       </c>
-      <c r="L47" s="1"/>
-      <c r="N47" s="1"/>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+      <c r="M48" s="1"/>
+      <c r="O48" s="1"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="F49" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F48" t="s">
+      <c r="G49" t="s">
         <v>138</v>
       </c>
-      <c r="L48" s="1"/>
-      <c r="N48" s="1"/>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="M49" s="1"/>
+      <c r="O49" s="1"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="F50" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F49" t="s">
+      <c r="G50" t="s">
         <v>139</v>
       </c>
-      <c r="L49" s="1"/>
-      <c r="N49" s="1"/>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="M50" s="1"/>
+      <c r="O50" s="1"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="F51" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F50" t="s">
+      <c r="G51" t="s">
         <v>140</v>
       </c>
-      <c r="L50" s="1"/>
-      <c r="N50" s="1"/>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="M51" s="1"/>
+      <c r="O51" s="1"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="F52" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F51" t="s">
+      <c r="G52" t="s">
         <v>141</v>
       </c>
-      <c r="L51" s="1"/>
-      <c r="N51" s="1"/>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="M52" s="1"/>
+      <c r="O52" s="1"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="F53" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F52" t="s">
+      <c r="G53" t="s">
         <v>142</v>
       </c>
-      <c r="L52" s="1"/>
-      <c r="N52" s="1"/>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="M53" s="1"/>
+      <c r="O53" s="1"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="F54" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F53" t="s">
+      <c r="G54" t="s">
         <v>143</v>
       </c>
-      <c r="L53" s="1"/>
-      <c r="N53" s="1"/>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+      <c r="M54" s="1"/>
+      <c r="O54" s="1"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="F55" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F54" t="s">
+      <c r="G55" t="s">
         <v>144</v>
       </c>
-      <c r="L54" s="1"/>
-      <c r="N54" s="1"/>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+      <c r="M55" s="1"/>
+      <c r="O55" s="1"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="F56" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F55" t="s">
+      <c r="G56" t="s">
         <v>146</v>
       </c>
-      <c r="L55" s="1"/>
-      <c r="N55" s="1"/>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+      <c r="M56" s="1"/>
+      <c r="O56" s="1"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="F57" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F56" t="s">
+      <c r="G57" t="s">
         <v>147</v>
       </c>
-      <c r="L56" s="1"/>
-      <c r="N56" s="1"/>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+      <c r="M57" s="1"/>
+      <c r="O57" s="1"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="F58" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F57" t="s">
+      <c r="G58" t="s">
         <v>148</v>
       </c>
-      <c r="L57" s="1"/>
-      <c r="N57" s="1"/>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+      <c r="M58" s="1"/>
+      <c r="O58" s="1"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="F59" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F58" t="s">
+      <c r="G59" t="s">
         <v>149</v>
       </c>
-      <c r="L58" s="1"/>
-      <c r="N58" s="1"/>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+      <c r="M59" s="1"/>
+      <c r="O59" s="1"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="F60" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F59" t="s">
+      <c r="G60" t="s">
         <v>150</v>
       </c>
-      <c r="L59" s="1"/>
-      <c r="N59" s="1"/>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+      <c r="M60" s="1"/>
+      <c r="O60" s="1"/>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="F61" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F60" t="s">
+      <c r="G61" t="s">
         <v>151</v>
       </c>
-      <c r="L60" s="1"/>
-      <c r="N60" s="1"/>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+      <c r="M61" s="1"/>
+      <c r="O61" s="1"/>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C62" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="F62" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F61" t="s">
+      <c r="G62" t="s">
         <v>152</v>
       </c>
-      <c r="L61" s="1"/>
-      <c r="N61" s="1"/>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+      <c r="M62" s="1"/>
+      <c r="O62" s="1"/>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="F63" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F62" t="s">
+      <c r="G63" t="s">
         <v>153</v>
       </c>
-      <c r="L62" s="1"/>
-      <c r="N62" s="1"/>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+      <c r="M63" s="1"/>
+      <c r="O63" s="1"/>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C64" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="F64" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F63" t="s">
+      <c r="G64" t="s">
         <v>154</v>
       </c>
-      <c r="L63" s="1"/>
-      <c r="N63" s="1"/>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+      <c r="M64" s="1"/>
+      <c r="O64" s="1"/>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C65" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="F65" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F64" t="s">
+      <c r="G65" t="s">
         <v>155</v>
       </c>
-      <c r="L64" s="1"/>
-      <c r="N64" s="1"/>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+      <c r="M65" s="1"/>
+      <c r="O65" s="1"/>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C66" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="E65" s="1" t="s">
+      <c r="F66" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F65" t="s">
+      <c r="G66" t="s">
         <v>156</v>
       </c>
-      <c r="L65" s="1"/>
-      <c r="N65" s="1"/>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+      <c r="M66" s="1"/>
+      <c r="O66" s="1"/>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="E66" s="1" t="s">
+      <c r="F67" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F66" t="s">
+      <c r="G67" t="s">
         <v>157</v>
       </c>
-      <c r="L66" s="1"/>
-      <c r="N66" s="1"/>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+      <c r="M67" s="1"/>
+      <c r="O67" s="1"/>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C68" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="E67" s="1" t="s">
+      <c r="F68" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F67" t="s">
+      <c r="G68" t="s">
         <v>158</v>
       </c>
-      <c r="L67" s="1"/>
-      <c r="N67" s="1"/>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+      <c r="M68" s="1"/>
+      <c r="O68" s="1"/>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C69" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="E68" s="1" t="s">
+      <c r="F69" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F68" t="s">
+      <c r="G69" t="s">
         <v>160</v>
       </c>
-      <c r="L68" s="1"/>
-      <c r="N68" s="1"/>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+      <c r="M69" s="1"/>
+      <c r="O69" s="1"/>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C70" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="E69" s="1" t="s">
+      <c r="F70" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F69" t="s">
+      <c r="G70" t="s">
         <v>161</v>
       </c>
-      <c r="L69" s="1"/>
-      <c r="N69" s="1"/>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+      <c r="M70" s="1"/>
+      <c r="O70" s="1"/>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C71" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="E70" s="1" t="s">
+      <c r="F71" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F70" t="s">
+      <c r="G71" t="s">
         <v>162</v>
       </c>
-      <c r="L70" s="1"/>
-      <c r="N70" s="1"/>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+      <c r="M71" s="1"/>
+      <c r="O71" s="1"/>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C72" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="E71" s="1" t="s">
+      <c r="F72" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F71" t="s">
+      <c r="G72" t="s">
         <v>163</v>
       </c>
-      <c r="L71" s="1"/>
-      <c r="N71" s="1"/>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+      <c r="M72" s="1"/>
+      <c r="O72" s="1"/>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C73" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="E72" s="1" t="s">
+      <c r="F73" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F72" t="s">
+      <c r="G73" t="s">
         <v>164</v>
       </c>
-      <c r="L72" s="1"/>
-      <c r="N72" s="1"/>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+      <c r="M73" s="1"/>
+      <c r="O73" s="1"/>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C74" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E73" s="1" t="s">
+      <c r="F74" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F73" t="s">
+      <c r="G74" t="s">
         <v>165</v>
       </c>
-      <c r="L73" s="1"/>
-      <c r="N73" s="1"/>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+      <c r="M74" s="1"/>
+      <c r="O74" s="1"/>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C75" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E74" s="1" t="s">
+      <c r="F75" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F74" t="s">
+      <c r="G75" t="s">
         <v>166</v>
       </c>
-      <c r="L74" s="1"/>
-      <c r="N74" s="1"/>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+      <c r="M75" s="1"/>
+      <c r="O75" s="1"/>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C76" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="E75" s="1" t="s">
+      <c r="F76" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F75" t="s">
+      <c r="G76" t="s">
         <v>167</v>
       </c>
-      <c r="L75" s="1"/>
-      <c r="N75" s="1"/>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+      <c r="M76" s="1"/>
+      <c r="O76" s="1"/>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C77" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E76" s="1" t="s">
+      <c r="F77" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F76" t="s">
+      <c r="G77" t="s">
         <v>168</v>
       </c>
-      <c r="L76" s="1"/>
-      <c r="N76" s="1"/>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+      <c r="M77" s="1"/>
+      <c r="O77" s="1"/>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C78" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="E77" s="1" t="s">
+      <c r="F78" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F77" t="s">
+      <c r="G78" t="s">
         <v>169</v>
       </c>
-      <c r="L77" s="1"/>
-      <c r="N77" s="1"/>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
+      <c r="M78" s="1"/>
+      <c r="O78" s="1"/>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C79" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="E78" s="1" t="s">
+      <c r="F79" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F78" t="s">
+      <c r="G79" t="s">
         <v>171</v>
       </c>
-      <c r="L78" s="1"/>
-      <c r="N78" s="1"/>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+      <c r="M79" s="1"/>
+      <c r="O79" s="1"/>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C80" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="E79" s="1" t="s">
+      <c r="F80" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F79" t="s">
+      <c r="G80" t="s">
         <v>172</v>
       </c>
-      <c r="L79" s="1"/>
-      <c r="N79" s="1"/>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+      <c r="M80" s="1"/>
+      <c r="O80" s="1"/>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C81" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="E80" s="1" t="s">
+      <c r="F81" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F80" t="s">
+      <c r="G81" t="s">
         <v>173</v>
       </c>
-      <c r="L80" s="1"/>
-      <c r="N80" s="1"/>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+      <c r="M81" s="1"/>
+      <c r="O81" s="1"/>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C82" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="E81" s="1" t="s">
+      <c r="F82" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F81" t="s">
+      <c r="G82" t="s">
         <v>174</v>
       </c>
-      <c r="L81" s="1"/>
-      <c r="N81" s="1"/>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+      <c r="M82" s="1"/>
+      <c r="O82" s="1"/>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C83" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="E82" s="1" t="s">
+      <c r="F83" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F82" t="s">
+      <c r="G83" t="s">
         <v>175</v>
       </c>
-      <c r="L82" s="1"/>
-      <c r="N82" s="1"/>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+      <c r="M83" s="1"/>
+      <c r="O83" s="1"/>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="E83" s="1" t="s">
+      <c r="F84" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F83" t="s">
+      <c r="G84" t="s">
         <v>176</v>
       </c>
-      <c r="L83" s="1"/>
-      <c r="N83" s="1"/>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+      <c r="M84" s="1"/>
+      <c r="O84" s="1"/>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C85" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="E84" s="1" t="s">
+      <c r="F85" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F84" t="s">
+      <c r="G85" t="s">
         <v>177</v>
       </c>
-      <c r="L84" s="1"/>
-      <c r="N84" s="1"/>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+      <c r="M85" s="1"/>
+      <c r="O85" s="1"/>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C86" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="E85" s="1" t="s">
+      <c r="F86" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F85" t="s">
+      <c r="G86" t="s">
         <v>178</v>
       </c>
-      <c r="L85" s="1"/>
-      <c r="N85" s="1"/>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+      <c r="M86" s="1"/>
+      <c r="O86" s="1"/>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C87" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="E86" s="1" t="s">
+      <c r="F87" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F86" t="s">
+      <c r="G87" t="s">
         <v>179</v>
       </c>
-      <c r="L86" s="1"/>
-      <c r="N86" s="1"/>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+      <c r="M87" s="1"/>
+      <c r="O87" s="1"/>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C88" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="E87" s="1" t="s">
+      <c r="F88" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F87" t="s">
+      <c r="G88" t="s">
         <v>180</v>
       </c>
-      <c r="L87" s="1"/>
-      <c r="N87" s="1"/>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+      <c r="M88" s="1"/>
+      <c r="O88" s="1"/>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C89" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E88" s="1" t="s">
+      <c r="F89" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="F88" t="s">
+      <c r="G89" t="s">
         <v>181</v>
       </c>
-      <c r="L88" s="1"/>
-      <c r="N88" s="1"/>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+      <c r="M89" s="1"/>
+      <c r="O89" s="1"/>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C90" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E89" s="1" t="s">
+      <c r="F90" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="F89" t="s">
+      <c r="G90" t="s">
         <v>183</v>
       </c>
-      <c r="L89" s="1"/>
-      <c r="N89" s="1"/>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
+      <c r="M90" s="1"/>
+      <c r="O90" s="1"/>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C91" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E90" s="1" t="s">
+      <c r="F91" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="F90" t="s">
+      <c r="G91" t="s">
         <v>184</v>
       </c>
-      <c r="L90" s="1"/>
-      <c r="N90" s="1"/>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+      <c r="M91" s="1"/>
+      <c r="O91" s="1"/>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C92" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E91" s="1" t="s">
+      <c r="F92" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="F91" t="s">
+      <c r="G92" t="s">
         <v>185</v>
       </c>
-      <c r="L91" s="1"/>
-      <c r="N91" s="1"/>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+      <c r="M92" s="1"/>
+      <c r="O92" s="1"/>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C93" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E92" s="1" t="s">
+      <c r="F93" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="F92" t="s">
+      <c r="G93" t="s">
         <v>186</v>
       </c>
-      <c r="L92" s="1"/>
-      <c r="N92" s="1"/>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+      <c r="M93" s="1"/>
+      <c r="O93" s="1"/>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C94" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E93" s="1" t="s">
+      <c r="F94" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="F93" t="s">
+      <c r="G94" t="s">
         <v>187</v>
       </c>
-      <c r="L93" s="1"/>
-      <c r="N93" s="1"/>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+      <c r="M94" s="1"/>
+      <c r="O94" s="1"/>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C95" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E94" s="1" t="s">
+      <c r="F95" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="F94" t="s">
+      <c r="G95" t="s">
         <v>188</v>
       </c>
-      <c r="L94" s="1"/>
-      <c r="N94" s="1"/>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
+      <c r="M95" s="1"/>
+      <c r="O95" s="1"/>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C96" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="E95" s="1" t="s">
+      <c r="F96" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="F95" t="s">
+      <c r="G96" t="s">
         <v>189</v>
       </c>
-      <c r="L95" s="1"/>
-      <c r="N95" s="1"/>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
+      <c r="M96" s="1"/>
+      <c r="O96" s="1"/>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="F96" t="s">
-        <v>190</v>
-      </c>
-      <c r="L96" s="1"/>
-      <c r="N96" s="1"/>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E97" s="1" t="s">
+      <c r="F97" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="F97" t="s">
+      <c r="G97" t="s">
         <v>190</v>
       </c>
-      <c r="L97" s="1"/>
-      <c r="N97" s="1"/>
-    </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M97" s="1"/>
+      <c r="O97" s="1"/>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G98" t="s">
+        <v>190</v>
+      </c>
+      <c r="M98" s="1"/>
+      <c r="O98" s="1"/>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="F98" t="s">
-        <v>192</v>
-      </c>
-      <c r="L98" s="1"/>
-      <c r="N98" s="1"/>
-    </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="E99" s="1" t="s">
+      <c r="F99" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="F99" t="s">
+      <c r="G99" t="s">
         <v>192</v>
       </c>
-      <c r="L99" s="1"/>
-      <c r="N99" s="1"/>
-    </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M99" s="1"/>
+      <c r="O99" s="1"/>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G100" t="s">
+        <v>192</v>
+      </c>
+      <c r="M100" s="1"/>
+      <c r="O100" s="1"/>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="F100" t="s">
-        <v>193</v>
-      </c>
-      <c r="L100" s="1"/>
-      <c r="N100" s="1"/>
-    </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>228</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E101" s="1" t="s">
+      <c r="F101" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="F101" t="s">
+      <c r="G101" t="s">
+        <v>193</v>
+      </c>
+      <c r="M101" s="1"/>
+      <c r="O101" s="1"/>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G102" t="s">
         <v>194</v>
       </c>
-      <c r="L101" s="1"/>
-      <c r="N101" s="1"/>
+      <c r="M102" s="1"/>
+      <c r="O102" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>